<commit_message>
add raw data loading for users, change readme
</commit_message>
<xml_diff>
--- a/var_naming.xlsx
+++ b/var_naming.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Dropbox\ПК\Desktop\giga_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF49B3A7-CDED-4C8C-AE50-47101A22C3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C01CA4E-E21E-4A0E-A5AC-A0313CEF858D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="870" windowWidth="25245" windowHeight="13455" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q" sheetId="1" r:id="rId1"/>
     <sheet name="m_rosstat" sheetId="2" r:id="rId2"/>
     <sheet name="m_fred" sheetId="3" r:id="rId3"/>
     <sheet name="m_cbr" sheetId="4" r:id="rId4"/>
+    <sheet name="all" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="162">
   <si>
     <t>ru_name</t>
   </si>
@@ -554,9 +555,6 @@
     <t>im_usd</t>
   </si>
   <si>
-    <t>https://www.cbr.ru/currency_base/dynamics/?UniDbQuery.Posted=True&amp;UniDbQuery.so=1&amp;UniDbQuery.mode=1&amp;UniDbQuery.date_req1=&amp;UniDbQuery.date_req2=&amp;UniDbQuery.VAL_NM_RQ=R01235&amp;UniDbQuery.From=01.01.1997&amp;UniDbQuery.To=22.10.2025</t>
-  </si>
-  <si>
     <t>ВВП в постоянных ценах</t>
   </si>
   <si>
@@ -579,13 +577,58 @@
   </si>
   <si>
     <t>inv_cap</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>sourse</t>
+  </si>
+  <si>
+    <t>Росстат</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/</t>
+  </si>
+  <si>
+    <t>Частота</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/MCOILBRENTEU</t>
+  </si>
+  <si>
+    <t>FRED</t>
+  </si>
+  <si>
+    <t>Номинальный эффективный обменный курс рубля</t>
+  </si>
+  <si>
+    <t>Реальный эффективный обменный курс рубля</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/RBRUBIS</t>
+  </si>
+  <si>
+    <t>Банк России</t>
+  </si>
+  <si>
+    <t>https://rosstat.gov.ru/statistics/accounts</t>
+  </si>
+  <si>
+    <t>https://fred.stlouisfed.org/series/NBRUBIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,6 +661,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -641,18 +692,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
     <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -932,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +999,7 @@
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -958,61 +1012,76 @@
       <c r="D1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" t="s">
-        <v>141</v>
       </c>
       <c r="D2">
         <v>1995</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D3">
         <v>1995</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D4">
         <v>1995</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
         <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>147</v>
       </c>
       <c r="D5">
         <v>1995</v>
+      </c>
+      <c r="E5" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1024,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA1632E-DF44-4A72-8632-363B974EBA5C}">
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F55" sqref="B1:F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1118,9 @@
       <c r="D1" t="s">
         <v>49</v>
       </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
       <c r="F1" t="s">
         <v>121</v>
       </c>
@@ -1066,6 +1138,9 @@
       <c r="D2">
         <v>1999</v>
       </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
       <c r="F2" t="s">
         <v>122</v>
       </c>
@@ -1083,6 +1158,9 @@
       <c r="D3">
         <v>1999</v>
       </c>
+      <c r="E3" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1097,6 +1175,9 @@
       <c r="D4">
         <v>1999</v>
       </c>
+      <c r="E4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1111,6 +1192,9 @@
       <c r="D5">
         <v>1999</v>
       </c>
+      <c r="E5" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1125,6 +1209,9 @@
       <c r="D6">
         <v>1999</v>
       </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1139,6 +1226,9 @@
       <c r="D7">
         <v>1999</v>
       </c>
+      <c r="E7" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1153,6 +1243,9 @@
       <c r="D8">
         <v>1999</v>
       </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1167,6 +1260,9 @@
       <c r="D9">
         <v>1999</v>
       </c>
+      <c r="E9" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1181,6 +1277,9 @@
       <c r="D10">
         <v>1999</v>
       </c>
+      <c r="E10" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1195,6 +1294,9 @@
       <c r="D11">
         <v>1999</v>
       </c>
+      <c r="E11" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1209,6 +1311,9 @@
       <c r="D12">
         <v>1999</v>
       </c>
+      <c r="E12" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1223,6 +1328,9 @@
       <c r="D13" s="2">
         <v>2005</v>
       </c>
+      <c r="E13" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1237,6 +1345,9 @@
       <c r="D14">
         <v>1999</v>
       </c>
+      <c r="E14" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1251,6 +1362,9 @@
       <c r="D15">
         <v>1999</v>
       </c>
+      <c r="E15" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1265,8 +1379,11 @@
       <c r="D16">
         <v>1999</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1279,8 +1396,11 @@
       <c r="D17">
         <v>1999</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1293,8 +1413,11 @@
       <c r="D18">
         <v>1999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1307,8 +1430,11 @@
       <c r="D19">
         <v>1999</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1321,8 +1447,11 @@
       <c r="D20">
         <v>1999</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1335,8 +1464,11 @@
       <c r="D21">
         <v>1999</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1349,8 +1481,11 @@
       <c r="D22">
         <v>1999</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1363,8 +1498,11 @@
       <c r="D23">
         <v>1999</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1377,8 +1515,11 @@
       <c r="D24">
         <v>1999</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1391,8 +1532,11 @@
       <c r="D25">
         <v>1999</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1405,8 +1549,11 @@
       <c r="D26" s="2">
         <v>2001</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1419,8 +1566,11 @@
       <c r="D27" s="2">
         <v>2001</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1433,8 +1583,11 @@
       <c r="D28">
         <v>1999</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1447,8 +1600,11 @@
       <c r="D29">
         <v>1999</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1461,8 +1617,11 @@
       <c r="D30">
         <v>1999</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1475,8 +1634,11 @@
       <c r="D31">
         <v>1999</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1489,8 +1651,11 @@
       <c r="D32">
         <v>1999</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1503,8 +1668,11 @@
       <c r="D33">
         <v>1999</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1517,8 +1685,11 @@
       <c r="D34">
         <v>1999</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1531,8 +1702,11 @@
       <c r="D35">
         <v>1999</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1545,8 +1719,11 @@
       <c r="D36">
         <v>1999</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1559,8 +1736,11 @@
       <c r="D37">
         <v>1999</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1573,8 +1753,11 @@
       <c r="D38">
         <v>1999</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1587,8 +1770,11 @@
       <c r="D39">
         <v>1999</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1601,8 +1787,11 @@
       <c r="D40">
         <v>1999</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1615,8 +1804,11 @@
       <c r="D41">
         <v>1999</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1629,8 +1821,11 @@
       <c r="D42">
         <v>1999</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1643,8 +1838,11 @@
       <c r="D43">
         <v>1999</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1657,8 +1855,11 @@
       <c r="D44">
         <v>1999</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1671,8 +1872,11 @@
       <c r="D45">
         <v>1999</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1685,8 +1889,11 @@
       <c r="D46">
         <v>1999</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1699,8 +1906,11 @@
       <c r="D47">
         <v>1999</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1713,8 +1923,11 @@
       <c r="D48">
         <v>1999</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1727,8 +1940,11 @@
       <c r="D49">
         <v>1999</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1741,8 +1957,11 @@
       <c r="D50">
         <v>1999</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1755,8 +1974,11 @@
       <c r="D51">
         <v>1999</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1769,8 +1991,11 @@
       <c r="D52">
         <v>1999</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1783,8 +2008,11 @@
       <c r="D53">
         <v>1999</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1797,8 +2025,11 @@
       <c r="D54">
         <v>1999</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1810,6 +2041,9 @@
       </c>
       <c r="D55">
         <v>1999</v>
+      </c>
+      <c r="E55" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1819,10 +2053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58507D29-C4B0-4D12-91A1-E423F2CF9436}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C4"/>
+      <selection sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,7 +2067,7 @@
     <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1849,8 +2083,11 @@
       <c r="E1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1866,8 +2103,11 @@
       <c r="E2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1883,8 +2123,11 @@
       <c r="E3" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1900,18 +2143,24 @@
       <c r="E4" t="s">
         <v>119</v>
       </c>
+      <c r="F4" t="s">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{F0A7949C-A263-4CEA-BDB4-D55D26DE6FAC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D98C75-3961-4D4F-9E20-2A7F58D75781}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +2185,7 @@
         <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>121</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2041,9 +2290,1590 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D0DC27-5A3D-47D2-91A8-239251A08FD9}">
+  <dimension ref="A1:G68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="66.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
         <v>139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2">
+        <v>1995</v>
+      </c>
+      <c r="F2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3">
+        <v>1995</v>
+      </c>
+      <c r="F3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4">
+        <v>1995</v>
+      </c>
+      <c r="F4" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5">
+        <v>1995</v>
+      </c>
+      <c r="F5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>1999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>1999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>1999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>1999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>1999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12">
+        <v>1999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13">
+        <v>1999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>1999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15">
+        <v>1999</v>
+      </c>
+      <c r="F15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16">
+        <v>1999</v>
+      </c>
+      <c r="F16" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2005</v>
+      </c>
+      <c r="F17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18">
+        <v>1999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19">
+        <v>1999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>149</v>
+      </c>
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20">
+        <v>1999</v>
+      </c>
+      <c r="F20" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>1999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>153</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>1999</v>
+      </c>
+      <c r="F22" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>153</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>1999</v>
+      </c>
+      <c r="F23" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24">
+        <v>1999</v>
+      </c>
+      <c r="F24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>1999</v>
+      </c>
+      <c r="F25" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26">
+        <v>1999</v>
+      </c>
+      <c r="F26" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27">
+        <v>1999</v>
+      </c>
+      <c r="F27" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28">
+        <v>1999</v>
+      </c>
+      <c r="F28" t="s">
+        <v>149</v>
+      </c>
+      <c r="G28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29">
+        <v>1999</v>
+      </c>
+      <c r="F29" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F30" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2001</v>
+      </c>
+      <c r="F31" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32">
+        <v>1999</v>
+      </c>
+      <c r="F32" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33">
+        <v>1999</v>
+      </c>
+      <c r="F33" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34">
+        <v>1999</v>
+      </c>
+      <c r="F34" t="s">
+        <v>149</v>
+      </c>
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35">
+        <v>1999</v>
+      </c>
+      <c r="F35" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36">
+        <v>1999</v>
+      </c>
+      <c r="F36" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37">
+        <v>1999</v>
+      </c>
+      <c r="F37" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38">
+        <v>1999</v>
+      </c>
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+      <c r="G38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>153</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39">
+        <v>1999</v>
+      </c>
+      <c r="F39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <v>1999</v>
+      </c>
+      <c r="F40" t="s">
+        <v>149</v>
+      </c>
+      <c r="G40" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41">
+        <v>1999</v>
+      </c>
+      <c r="F41" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42">
+        <v>1999</v>
+      </c>
+      <c r="F42" t="s">
+        <v>149</v>
+      </c>
+      <c r="G42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43">
+        <v>1999</v>
+      </c>
+      <c r="F43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>153</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44">
+        <v>1999</v>
+      </c>
+      <c r="F44" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45">
+        <v>1999</v>
+      </c>
+      <c r="F45" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46">
+        <v>1999</v>
+      </c>
+      <c r="F46" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47">
+        <v>1999</v>
+      </c>
+      <c r="F47" t="s">
+        <v>149</v>
+      </c>
+      <c r="G47" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" t="s">
+        <v>81</v>
+      </c>
+      <c r="E48">
+        <v>1999</v>
+      </c>
+      <c r="F48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>153</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" t="s">
+        <v>82</v>
+      </c>
+      <c r="E49">
+        <v>1999</v>
+      </c>
+      <c r="F49" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50">
+        <v>1999</v>
+      </c>
+      <c r="F50" t="s">
+        <v>149</v>
+      </c>
+      <c r="G50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>153</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" t="s">
+        <v>84</v>
+      </c>
+      <c r="E51">
+        <v>1999</v>
+      </c>
+      <c r="F51" t="s">
+        <v>149</v>
+      </c>
+      <c r="G51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D52" t="s">
+        <v>88</v>
+      </c>
+      <c r="E52">
+        <v>1999</v>
+      </c>
+      <c r="F52" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>153</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53">
+        <v>1999</v>
+      </c>
+      <c r="F53" t="s">
+        <v>149</v>
+      </c>
+      <c r="G53" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+      <c r="E54">
+        <v>1999</v>
+      </c>
+      <c r="F54" t="s">
+        <v>149</v>
+      </c>
+      <c r="G54" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D55" t="s">
+        <v>102</v>
+      </c>
+      <c r="E55">
+        <v>1999</v>
+      </c>
+      <c r="F55" t="s">
+        <v>149</v>
+      </c>
+      <c r="G55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>153</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D56" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56">
+        <v>1999</v>
+      </c>
+      <c r="F56" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" t="s">
+        <v>104</v>
+      </c>
+      <c r="E57">
+        <v>1999</v>
+      </c>
+      <c r="F57" t="s">
+        <v>149</v>
+      </c>
+      <c r="G57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D58" t="s">
+        <v>107</v>
+      </c>
+      <c r="E58">
+        <v>1999</v>
+      </c>
+      <c r="F58" t="s">
+        <v>149</v>
+      </c>
+      <c r="G58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>153</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" t="s">
+        <v>108</v>
+      </c>
+      <c r="E59">
+        <v>1999</v>
+      </c>
+      <c r="F59" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>153</v>
+      </c>
+      <c r="C60" t="s">
+        <v>111</v>
+      </c>
+      <c r="D60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60">
+        <v>1999</v>
+      </c>
+      <c r="F60" t="s">
+        <v>155</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" t="s">
+        <v>117</v>
+      </c>
+      <c r="E61">
+        <v>1999</v>
+      </c>
+      <c r="F61" t="s">
+        <v>155</v>
+      </c>
+      <c r="G61" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>153</v>
+      </c>
+      <c r="C62" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" t="s">
+        <v>118</v>
+      </c>
+      <c r="E62">
+        <v>1999</v>
+      </c>
+      <c r="F62" t="s">
+        <v>155</v>
+      </c>
+      <c r="G62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>153</v>
+      </c>
+      <c r="C63" t="s">
+        <v>123</v>
+      </c>
+      <c r="D63" t="s">
+        <v>124</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F63" t="s">
+        <v>159</v>
+      </c>
+      <c r="G63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>153</v>
+      </c>
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+      <c r="D64" t="s">
+        <v>128</v>
+      </c>
+      <c r="E64">
+        <v>2001</v>
+      </c>
+      <c r="F64" t="s">
+        <v>159</v>
+      </c>
+      <c r="G64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" t="s">
+        <v>133</v>
+      </c>
+      <c r="D65" t="s">
+        <v>129</v>
+      </c>
+      <c r="E65">
+        <v>2001</v>
+      </c>
+      <c r="F65" t="s">
+        <v>159</v>
+      </c>
+      <c r="G65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" t="s">
+        <v>134</v>
+      </c>
+      <c r="D66" t="s">
+        <v>130</v>
+      </c>
+      <c r="E66">
+        <v>2001</v>
+      </c>
+      <c r="F66" t="s">
+        <v>159</v>
+      </c>
+      <c r="G66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" t="s">
+        <v>137</v>
+      </c>
+      <c r="E67">
+        <v>1997</v>
+      </c>
+      <c r="F67" t="s">
+        <v>159</v>
+      </c>
+      <c r="G67" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>153</v>
+      </c>
+      <c r="C68" t="s">
+        <v>136</v>
+      </c>
+      <c r="D68" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68">
+        <v>1997</v>
+      </c>
+      <c r="F68" t="s">
+        <v>159</v>
+      </c>
+      <c r="G68" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>